<commit_message>
Add problem statement and SQL script for removing outliers in hotel ratings
</commit_message>
<xml_diff>
--- a/Remove_Outliers/Problem_Statement.xlsx
+++ b/Remove_Outliers/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q11/Video_Q11_Scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Remove_Outliers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B4CB83-9846-1A4E-B02B-3C7B48429734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EA5F2E-2E52-43B4-BBDD-297AEAAB65F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{22AEC6DC-9F68-BF49-A715-6DB72E91B044}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{22AEC6DC-9F68-BF49-A715-6DB72E91B044}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -59,29 +57,6 @@
     <r>
       <rPr>
         <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Video #11</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - Remove Outliers</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
         <u/>
         <sz val="12"/>
         <color theme="0"/>
@@ -99,6 +74,29 @@
       </rPr>
       <t xml:space="preserve"> In the given input table, there are hotel ratings which are either too high or too low compared to the standard ratings the hotel receives each year. Write a query to identify and exclude these outlier records as shown in expected output below. 
 Your output should follow the same order of records as shown.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Remove Outliers</t>
     </r>
   </si>
 </sst>
@@ -792,23 +790,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B14727-820F-4547-A39B-7446BCA17713}">
   <dimension ref="B1:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="15.83203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="15.83203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="2" width="15.796875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" style="1"/>
+    <col min="6" max="6" width="15.796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="B1" s="23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -817,9 +815,9 @@
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
     </row>
-    <row r="2" spans="2:8" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" s="3" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -828,7 +826,7 @@
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
     </row>
-    <row r="3" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -837,7 +835,7 @@
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -846,7 +844,7 @@
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -855,8 +853,8 @@
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="7" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="20" t="s">
         <v>5</v>
       </c>
@@ -868,7 +866,7 @@
       <c r="G8" s="21"/>
       <c r="H8" s="22"/>
     </row>
-    <row r="9" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="16" t="s">
         <v>2</v>
       </c>
@@ -888,7 +886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>0</v>
       </c>
@@ -908,7 +906,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>0</v>
       </c>
@@ -928,7 +926,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>0</v>
       </c>
@@ -948,7 +946,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
@@ -968,7 +966,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
@@ -988,7 +986,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>1</v>
       </c>
@@ -1008,7 +1006,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1017,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7" t="s">
         <v>1</v>
       </c>
@@ -1038,5 +1036,6 @@
     <mergeCell ref="B2:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>